<commit_message>
Captura URL e redireciona para ela ao salvar o adverso... programando o looping
</commit_message>
<xml_diff>
--- a/teste_db.xlsx
+++ b/teste_db.xlsx
@@ -84,9 +84,6 @@
     <t>Grupo 4</t>
   </si>
   <si>
-    <t>ABIGAIL MAIA DA SILVA</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>PA</t>
   </si>
   <si>
-    <t>ABRAAO VIEIRA DA COSTA</t>
-  </si>
-  <si>
     <t>Porto Velho</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>RO</t>
   </si>
   <si>
-    <t>ACACIO FERNANDES DE SOUZA</t>
-  </si>
-  <si>
     <t>Ariquemes</t>
   </si>
   <si>
@@ -124,6 +115,15 @@
   </si>
   <si>
     <t>2 ª-º;Vara Cível</t>
+  </si>
+  <si>
+    <t>ABIGAIL MAIA DA SILVA 20</t>
+  </si>
+  <si>
+    <t>ABRAAO VIEIRA DA COSTA 20</t>
+  </si>
+  <si>
+    <t>ACACIO FERNANDES DE SOUZA 20</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1077,7 @@
     <col min="7" max="7" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1169,19 +1169,19 @@
         <v>20</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="O2" s="8">
         <v>10314.299999999999</v>
@@ -1190,7 +1190,7 @@
         <v>43238</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1221,19 +1221,19 @@
         <v>20</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="O3" s="8">
         <v>10000</v>
@@ -1242,7 +1242,7 @@
         <v>43083</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1273,19 +1273,19 @@
         <v>20</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O4" s="8">
         <v>38621.82</v>
@@ -1294,7 +1294,7 @@
         <v>42801</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>